<commit_message>
modify database on message kv save
</commit_message>
<xml_diff>
--- a/config/excel/DataBase.xlsx
+++ b/config/excel/DataBase.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proj\demo1\config\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proj\server_demo\config\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA61DBF1-4D59-4E70-8E1E-0647A89CBB59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
   </bookViews>
   <sheets>
     <sheet name="DataBase" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -82,10 +81,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>IP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Port</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -95,13 +90,25 @@
   </si>
   <si>
     <t>Password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rocksdb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/data/db</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -419,11 +426,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -482,16 +489,16 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -512,6 +519,17 @@
       </c>
       <c r="F5">
         <v>123456</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>10002</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>